<commit_message>
Add ADT price calculation and configurable Excel export
- Integrated ADT price calculation into Product model
- Combined ADT results with base results in the same Excel file (side by side instead of overwrite)
- Added support for custom output filename and location in Product class
</commit_message>
<xml_diff>
--- a/business-card.xlsx
+++ b/business-card.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:S71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,6 +474,61 @@
           <t>tirazh</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>AdtPrice</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>workTypeID</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>deliveryID</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>sampleSizeID</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>sampleID</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>multiCopyCount</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>sampleMaterialID</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>samplePrintKindID</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>side</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>tirazhCount</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -500,6 +555,39 @@
       <c r="H2" t="n">
         <v>1</v>
       </c>
+      <c r="I2" t="n">
+        <v>3989</v>
+      </c>
+      <c r="J2" t="n">
+        <v>3</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L2" t="n">
+        <v>288</v>
+      </c>
+      <c r="M2" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>15889</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -526,6 +614,39 @@
       <c r="H3" t="n">
         <v>50</v>
       </c>
+      <c r="I3" t="n">
+        <v>98100</v>
+      </c>
+      <c r="J3" t="n">
+        <v>3</v>
+      </c>
+      <c r="K3" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L3" t="n">
+        <v>288</v>
+      </c>
+      <c r="M3" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P3" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>15889</v>
+      </c>
+      <c r="R3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S3" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -552,6 +673,39 @@
       <c r="H4" t="n">
         <v>100</v>
       </c>
+      <c r="I4" t="n">
+        <v>173600</v>
+      </c>
+      <c r="J4" t="n">
+        <v>3</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L4" t="n">
+        <v>288</v>
+      </c>
+      <c r="M4" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P4" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>15889</v>
+      </c>
+      <c r="R4" t="n">
+        <v>1</v>
+      </c>
+      <c r="S4" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -578,6 +732,39 @@
       <c r="H5" t="n">
         <v>200</v>
       </c>
+      <c r="I5" t="n">
+        <v>322200</v>
+      </c>
+      <c r="J5" t="n">
+        <v>3</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L5" t="n">
+        <v>288</v>
+      </c>
+      <c r="M5" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P5" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>15889</v>
+      </c>
+      <c r="R5" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -604,6 +791,39 @@
       <c r="H6" t="n">
         <v>300</v>
       </c>
+      <c r="I6" t="n">
+        <v>449700</v>
+      </c>
+      <c r="J6" t="n">
+        <v>3</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L6" t="n">
+        <v>288</v>
+      </c>
+      <c r="M6" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P6" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>15889</v>
+      </c>
+      <c r="R6" t="n">
+        <v>1</v>
+      </c>
+      <c r="S6" t="n">
+        <v>300</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -630,6 +850,39 @@
       <c r="H7" t="n">
         <v>500</v>
       </c>
+      <c r="I7" t="n">
+        <v>673000</v>
+      </c>
+      <c r="J7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L7" t="n">
+        <v>288</v>
+      </c>
+      <c r="M7" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1</v>
+      </c>
+      <c r="O7" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P7" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>15889</v>
+      </c>
+      <c r="R7" t="n">
+        <v>1</v>
+      </c>
+      <c r="S7" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -656,6 +909,39 @@
       <c r="H8" t="n">
         <v>1000</v>
       </c>
+      <c r="I8" t="n">
+        <v>1339000</v>
+      </c>
+      <c r="J8" t="n">
+        <v>3</v>
+      </c>
+      <c r="K8" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L8" t="n">
+        <v>288</v>
+      </c>
+      <c r="M8" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N8" t="n">
+        <v>1</v>
+      </c>
+      <c r="O8" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P8" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>15889</v>
+      </c>
+      <c r="R8" t="n">
+        <v>1</v>
+      </c>
+      <c r="S8" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -682,6 +968,39 @@
       <c r="H9" t="n">
         <v>1</v>
       </c>
+      <c r="I9" t="n">
+        <v>6396</v>
+      </c>
+      <c r="J9" t="n">
+        <v>3</v>
+      </c>
+      <c r="K9" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L9" t="n">
+        <v>288</v>
+      </c>
+      <c r="M9" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1</v>
+      </c>
+      <c r="O9" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P9" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>15889</v>
+      </c>
+      <c r="R9" t="n">
+        <v>2</v>
+      </c>
+      <c r="S9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -708,6 +1027,39 @@
       <c r="H10" t="n">
         <v>50</v>
       </c>
+      <c r="I10" t="n">
+        <v>206500</v>
+      </c>
+      <c r="J10" t="n">
+        <v>3</v>
+      </c>
+      <c r="K10" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L10" t="n">
+        <v>288</v>
+      </c>
+      <c r="M10" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N10" t="n">
+        <v>1</v>
+      </c>
+      <c r="O10" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P10" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>15889</v>
+      </c>
+      <c r="R10" t="n">
+        <v>2</v>
+      </c>
+      <c r="S10" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -734,6 +1086,39 @@
       <c r="H11" t="n">
         <v>100</v>
       </c>
+      <c r="I11" t="n">
+        <v>363300</v>
+      </c>
+      <c r="J11" t="n">
+        <v>3</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L11" t="n">
+        <v>288</v>
+      </c>
+      <c r="M11" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P11" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>15889</v>
+      </c>
+      <c r="R11" t="n">
+        <v>2</v>
+      </c>
+      <c r="S11" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -760,6 +1145,39 @@
       <c r="H12" t="n">
         <v>200</v>
       </c>
+      <c r="I12" t="n">
+        <v>685800</v>
+      </c>
+      <c r="J12" t="n">
+        <v>3</v>
+      </c>
+      <c r="K12" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L12" t="n">
+        <v>288</v>
+      </c>
+      <c r="M12" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N12" t="n">
+        <v>1</v>
+      </c>
+      <c r="O12" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P12" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>15889</v>
+      </c>
+      <c r="R12" t="n">
+        <v>2</v>
+      </c>
+      <c r="S12" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -786,6 +1204,39 @@
       <c r="H13" t="n">
         <v>300</v>
       </c>
+      <c r="I13" t="n">
+        <v>952500</v>
+      </c>
+      <c r="J13" t="n">
+        <v>3</v>
+      </c>
+      <c r="K13" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L13" t="n">
+        <v>288</v>
+      </c>
+      <c r="M13" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N13" t="n">
+        <v>1</v>
+      </c>
+      <c r="O13" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P13" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>15889</v>
+      </c>
+      <c r="R13" t="n">
+        <v>2</v>
+      </c>
+      <c r="S13" t="n">
+        <v>300</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -812,6 +1263,39 @@
       <c r="H14" t="n">
         <v>500</v>
       </c>
+      <c r="I14" t="n">
+        <v>1461000</v>
+      </c>
+      <c r="J14" t="n">
+        <v>3</v>
+      </c>
+      <c r="K14" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L14" t="n">
+        <v>288</v>
+      </c>
+      <c r="M14" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N14" t="n">
+        <v>1</v>
+      </c>
+      <c r="O14" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P14" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>15889</v>
+      </c>
+      <c r="R14" t="n">
+        <v>2</v>
+      </c>
+      <c r="S14" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -838,6 +1322,39 @@
       <c r="H15" t="n">
         <v>1000</v>
       </c>
+      <c r="I15" t="n">
+        <v>2722000</v>
+      </c>
+      <c r="J15" t="n">
+        <v>3</v>
+      </c>
+      <c r="K15" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L15" t="n">
+        <v>288</v>
+      </c>
+      <c r="M15" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N15" t="n">
+        <v>1</v>
+      </c>
+      <c r="O15" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P15" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>15889</v>
+      </c>
+      <c r="R15" t="n">
+        <v>2</v>
+      </c>
+      <c r="S15" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -864,6 +1381,39 @@
       <c r="H16" t="n">
         <v>1</v>
       </c>
+      <c r="I16" t="n">
+        <v>3874</v>
+      </c>
+      <c r="J16" t="n">
+        <v>3</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L16" t="n">
+        <v>288</v>
+      </c>
+      <c r="M16" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N16" t="n">
+        <v>1</v>
+      </c>
+      <c r="O16" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P16" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>15890</v>
+      </c>
+      <c r="R16" t="n">
+        <v>1</v>
+      </c>
+      <c r="S16" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -890,6 +1440,39 @@
       <c r="H17" t="n">
         <v>50</v>
       </c>
+      <c r="I17" t="n">
+        <v>95250</v>
+      </c>
+      <c r="J17" t="n">
+        <v>3</v>
+      </c>
+      <c r="K17" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L17" t="n">
+        <v>288</v>
+      </c>
+      <c r="M17" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O17" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P17" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>15890</v>
+      </c>
+      <c r="R17" t="n">
+        <v>1</v>
+      </c>
+      <c r="S17" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -916,6 +1499,39 @@
       <c r="H18" t="n">
         <v>100</v>
       </c>
+      <c r="I18" t="n">
+        <v>167900</v>
+      </c>
+      <c r="J18" t="n">
+        <v>3</v>
+      </c>
+      <c r="K18" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L18" t="n">
+        <v>288</v>
+      </c>
+      <c r="M18" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N18" t="n">
+        <v>1</v>
+      </c>
+      <c r="O18" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P18" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>15890</v>
+      </c>
+      <c r="R18" t="n">
+        <v>1</v>
+      </c>
+      <c r="S18" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -942,6 +1558,39 @@
       <c r="H19" t="n">
         <v>200</v>
       </c>
+      <c r="I19" t="n">
+        <v>314400</v>
+      </c>
+      <c r="J19" t="n">
+        <v>3</v>
+      </c>
+      <c r="K19" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L19" t="n">
+        <v>288</v>
+      </c>
+      <c r="M19" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N19" t="n">
+        <v>1</v>
+      </c>
+      <c r="O19" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P19" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>15890</v>
+      </c>
+      <c r="R19" t="n">
+        <v>1</v>
+      </c>
+      <c r="S19" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -968,6 +1617,39 @@
       <c r="H20" t="n">
         <v>300</v>
       </c>
+      <c r="I20" t="n">
+        <v>437400</v>
+      </c>
+      <c r="J20" t="n">
+        <v>3</v>
+      </c>
+      <c r="K20" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L20" t="n">
+        <v>288</v>
+      </c>
+      <c r="M20" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O20" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P20" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>15890</v>
+      </c>
+      <c r="R20" t="n">
+        <v>1</v>
+      </c>
+      <c r="S20" t="n">
+        <v>300</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -994,6 +1676,39 @@
       <c r="H21" t="n">
         <v>500</v>
       </c>
+      <c r="I21" t="n">
+        <v>660500</v>
+      </c>
+      <c r="J21" t="n">
+        <v>3</v>
+      </c>
+      <c r="K21" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L21" t="n">
+        <v>288</v>
+      </c>
+      <c r="M21" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O21" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P21" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>15890</v>
+      </c>
+      <c r="R21" t="n">
+        <v>1</v>
+      </c>
+      <c r="S21" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1020,6 +1735,39 @@
       <c r="H22" t="n">
         <v>1000</v>
       </c>
+      <c r="I22" t="n">
+        <v>1302000</v>
+      </c>
+      <c r="J22" t="n">
+        <v>3</v>
+      </c>
+      <c r="K22" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L22" t="n">
+        <v>288</v>
+      </c>
+      <c r="M22" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N22" t="n">
+        <v>1</v>
+      </c>
+      <c r="O22" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P22" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>15890</v>
+      </c>
+      <c r="R22" t="n">
+        <v>1</v>
+      </c>
+      <c r="S22" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1046,6 +1794,39 @@
       <c r="H23" t="n">
         <v>1</v>
       </c>
+      <c r="I23" t="n">
+        <v>6198</v>
+      </c>
+      <c r="J23" t="n">
+        <v>3</v>
+      </c>
+      <c r="K23" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L23" t="n">
+        <v>288</v>
+      </c>
+      <c r="M23" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N23" t="n">
+        <v>1</v>
+      </c>
+      <c r="O23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P23" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>15890</v>
+      </c>
+      <c r="R23" t="n">
+        <v>2</v>
+      </c>
+      <c r="S23" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1072,6 +1853,39 @@
       <c r="H24" t="n">
         <v>50</v>
       </c>
+      <c r="I24" t="n">
+        <v>200300</v>
+      </c>
+      <c r="J24" t="n">
+        <v>3</v>
+      </c>
+      <c r="K24" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L24" t="n">
+        <v>288</v>
+      </c>
+      <c r="M24" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N24" t="n">
+        <v>1</v>
+      </c>
+      <c r="O24" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P24" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>15890</v>
+      </c>
+      <c r="R24" t="n">
+        <v>2</v>
+      </c>
+      <c r="S24" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1098,6 +1912,39 @@
       <c r="H25" t="n">
         <v>100</v>
       </c>
+      <c r="I25" t="n">
+        <v>353000</v>
+      </c>
+      <c r="J25" t="n">
+        <v>3</v>
+      </c>
+      <c r="K25" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L25" t="n">
+        <v>288</v>
+      </c>
+      <c r="M25" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N25" t="n">
+        <v>1</v>
+      </c>
+      <c r="O25" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P25" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>15890</v>
+      </c>
+      <c r="R25" t="n">
+        <v>2</v>
+      </c>
+      <c r="S25" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1124,6 +1971,39 @@
       <c r="H26" t="n">
         <v>200</v>
       </c>
+      <c r="I26" t="n">
+        <v>664600</v>
+      </c>
+      <c r="J26" t="n">
+        <v>3</v>
+      </c>
+      <c r="K26" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L26" t="n">
+        <v>288</v>
+      </c>
+      <c r="M26" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N26" t="n">
+        <v>1</v>
+      </c>
+      <c r="O26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P26" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>15890</v>
+      </c>
+      <c r="R26" t="n">
+        <v>2</v>
+      </c>
+      <c r="S26" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1150,6 +2030,39 @@
       <c r="H27" t="n">
         <v>300</v>
       </c>
+      <c r="I27" t="n">
+        <v>922800</v>
+      </c>
+      <c r="J27" t="n">
+        <v>3</v>
+      </c>
+      <c r="K27" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L27" t="n">
+        <v>288</v>
+      </c>
+      <c r="M27" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O27" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P27" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>15890</v>
+      </c>
+      <c r="R27" t="n">
+        <v>2</v>
+      </c>
+      <c r="S27" t="n">
+        <v>300</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1176,6 +2089,39 @@
       <c r="H28" t="n">
         <v>500</v>
       </c>
+      <c r="I28" t="n">
+        <v>1416000</v>
+      </c>
+      <c r="J28" t="n">
+        <v>3</v>
+      </c>
+      <c r="K28" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L28" t="n">
+        <v>288</v>
+      </c>
+      <c r="M28" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N28" t="n">
+        <v>1</v>
+      </c>
+      <c r="O28" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P28" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>15890</v>
+      </c>
+      <c r="R28" t="n">
+        <v>2</v>
+      </c>
+      <c r="S28" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1202,6 +2148,39 @@
       <c r="H29" t="n">
         <v>1000</v>
       </c>
+      <c r="I29" t="n">
+        <v>2640000</v>
+      </c>
+      <c r="J29" t="n">
+        <v>3</v>
+      </c>
+      <c r="K29" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L29" t="n">
+        <v>288</v>
+      </c>
+      <c r="M29" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N29" t="n">
+        <v>1</v>
+      </c>
+      <c r="O29" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P29" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>15890</v>
+      </c>
+      <c r="R29" t="n">
+        <v>2</v>
+      </c>
+      <c r="S29" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1228,6 +2207,39 @@
       <c r="H30" t="n">
         <v>1</v>
       </c>
+      <c r="I30" t="n">
+        <v>6195</v>
+      </c>
+      <c r="J30" t="n">
+        <v>3</v>
+      </c>
+      <c r="K30" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L30" t="n">
+        <v>288</v>
+      </c>
+      <c r="M30" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N30" t="n">
+        <v>1</v>
+      </c>
+      <c r="O30" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P30" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>15891</v>
+      </c>
+      <c r="R30" t="n">
+        <v>1</v>
+      </c>
+      <c r="S30" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1254,6 +2266,39 @@
       <c r="H31" t="n">
         <v>50</v>
       </c>
+      <c r="I31" t="n">
+        <v>235100</v>
+      </c>
+      <c r="J31" t="n">
+        <v>3</v>
+      </c>
+      <c r="K31" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L31" t="n">
+        <v>288</v>
+      </c>
+      <c r="M31" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N31" t="n">
+        <v>1</v>
+      </c>
+      <c r="O31" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P31" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>15891</v>
+      </c>
+      <c r="R31" t="n">
+        <v>1</v>
+      </c>
+      <c r="S31" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1280,6 +2325,39 @@
       <c r="H32" t="n">
         <v>100</v>
       </c>
+      <c r="I32" t="n">
+        <v>438200</v>
+      </c>
+      <c r="J32" t="n">
+        <v>3</v>
+      </c>
+      <c r="K32" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L32" t="n">
+        <v>288</v>
+      </c>
+      <c r="M32" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N32" t="n">
+        <v>1</v>
+      </c>
+      <c r="O32" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P32" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>15891</v>
+      </c>
+      <c r="R32" t="n">
+        <v>1</v>
+      </c>
+      <c r="S32" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1306,6 +2384,39 @@
       <c r="H33" t="n">
         <v>200</v>
       </c>
+      <c r="I33" t="n">
+        <v>846800</v>
+      </c>
+      <c r="J33" t="n">
+        <v>3</v>
+      </c>
+      <c r="K33" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L33" t="n">
+        <v>288</v>
+      </c>
+      <c r="M33" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N33" t="n">
+        <v>1</v>
+      </c>
+      <c r="O33" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P33" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>15891</v>
+      </c>
+      <c r="R33" t="n">
+        <v>1</v>
+      </c>
+      <c r="S33" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1332,6 +2443,39 @@
       <c r="H34" t="n">
         <v>300</v>
       </c>
+      <c r="I34" t="n">
+        <v>1244100</v>
+      </c>
+      <c r="J34" t="n">
+        <v>3</v>
+      </c>
+      <c r="K34" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L34" t="n">
+        <v>288</v>
+      </c>
+      <c r="M34" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N34" t="n">
+        <v>1</v>
+      </c>
+      <c r="O34" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P34" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>15891</v>
+      </c>
+      <c r="R34" t="n">
+        <v>1</v>
+      </c>
+      <c r="S34" t="n">
+        <v>300</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -1358,6 +2502,39 @@
       <c r="H35" t="n">
         <v>500</v>
       </c>
+      <c r="I35" t="n">
+        <v>1990500</v>
+      </c>
+      <c r="J35" t="n">
+        <v>3</v>
+      </c>
+      <c r="K35" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L35" t="n">
+        <v>288</v>
+      </c>
+      <c r="M35" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N35" t="n">
+        <v>1</v>
+      </c>
+      <c r="O35" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P35" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>15891</v>
+      </c>
+      <c r="R35" t="n">
+        <v>1</v>
+      </c>
+      <c r="S35" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -1384,6 +2561,39 @@
       <c r="H36" t="n">
         <v>1000</v>
       </c>
+      <c r="I36" t="n">
+        <v>3844000</v>
+      </c>
+      <c r="J36" t="n">
+        <v>3</v>
+      </c>
+      <c r="K36" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L36" t="n">
+        <v>288</v>
+      </c>
+      <c r="M36" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N36" t="n">
+        <v>1</v>
+      </c>
+      <c r="O36" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P36" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>15891</v>
+      </c>
+      <c r="R36" t="n">
+        <v>1</v>
+      </c>
+      <c r="S36" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1410,6 +2620,39 @@
       <c r="H37" t="n">
         <v>1</v>
       </c>
+      <c r="I37" t="n">
+        <v>7782</v>
+      </c>
+      <c r="J37" t="n">
+        <v>3</v>
+      </c>
+      <c r="K37" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L37" t="n">
+        <v>288</v>
+      </c>
+      <c r="M37" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N37" t="n">
+        <v>1</v>
+      </c>
+      <c r="O37" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P37" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>15891</v>
+      </c>
+      <c r="R37" t="n">
+        <v>2</v>
+      </c>
+      <c r="S37" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -1436,6 +2679,39 @@
       <c r="H38" t="n">
         <v>50</v>
       </c>
+      <c r="I38" t="n">
+        <v>476500</v>
+      </c>
+      <c r="J38" t="n">
+        <v>3</v>
+      </c>
+      <c r="K38" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L38" t="n">
+        <v>288</v>
+      </c>
+      <c r="M38" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N38" t="n">
+        <v>1</v>
+      </c>
+      <c r="O38" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P38" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>15891</v>
+      </c>
+      <c r="R38" t="n">
+        <v>2</v>
+      </c>
+      <c r="S38" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -1462,6 +2738,39 @@
       <c r="H39" t="n">
         <v>100</v>
       </c>
+      <c r="I39" t="n">
+        <v>887800</v>
+      </c>
+      <c r="J39" t="n">
+        <v>3</v>
+      </c>
+      <c r="K39" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L39" t="n">
+        <v>288</v>
+      </c>
+      <c r="M39" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N39" t="n">
+        <v>1</v>
+      </c>
+      <c r="O39" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P39" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>15891</v>
+      </c>
+      <c r="R39" t="n">
+        <v>2</v>
+      </c>
+      <c r="S39" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -1488,6 +2797,39 @@
       <c r="H40" t="n">
         <v>200</v>
       </c>
+      <c r="I40" t="n">
+        <v>1713200</v>
+      </c>
+      <c r="J40" t="n">
+        <v>3</v>
+      </c>
+      <c r="K40" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L40" t="n">
+        <v>288</v>
+      </c>
+      <c r="M40" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N40" t="n">
+        <v>1</v>
+      </c>
+      <c r="O40" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P40" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>15891</v>
+      </c>
+      <c r="R40" t="n">
+        <v>2</v>
+      </c>
+      <c r="S40" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -1514,6 +2856,39 @@
       <c r="H41" t="n">
         <v>300</v>
       </c>
+      <c r="I41" t="n">
+        <v>2479200</v>
+      </c>
+      <c r="J41" t="n">
+        <v>3</v>
+      </c>
+      <c r="K41" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L41" t="n">
+        <v>288</v>
+      </c>
+      <c r="M41" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N41" t="n">
+        <v>1</v>
+      </c>
+      <c r="O41" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P41" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>15891</v>
+      </c>
+      <c r="R41" t="n">
+        <v>2</v>
+      </c>
+      <c r="S41" t="n">
+        <v>300</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -1540,6 +2915,39 @@
       <c r="H42" t="n">
         <v>500</v>
       </c>
+      <c r="I42" t="n">
+        <v>3975500</v>
+      </c>
+      <c r="J42" t="n">
+        <v>3</v>
+      </c>
+      <c r="K42" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L42" t="n">
+        <v>288</v>
+      </c>
+      <c r="M42" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N42" t="n">
+        <v>1</v>
+      </c>
+      <c r="O42" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P42" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>15891</v>
+      </c>
+      <c r="R42" t="n">
+        <v>2</v>
+      </c>
+      <c r="S42" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -1566,6 +2974,39 @@
       <c r="H43" t="n">
         <v>1000</v>
       </c>
+      <c r="I43" t="n">
+        <v>7623000</v>
+      </c>
+      <c r="J43" t="n">
+        <v>3</v>
+      </c>
+      <c r="K43" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L43" t="n">
+        <v>288</v>
+      </c>
+      <c r="M43" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N43" t="n">
+        <v>1</v>
+      </c>
+      <c r="O43" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P43" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>15891</v>
+      </c>
+      <c r="R43" t="n">
+        <v>2</v>
+      </c>
+      <c r="S43" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -1592,6 +3033,39 @@
       <c r="H44" t="n">
         <v>1</v>
       </c>
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" t="n">
+        <v>3</v>
+      </c>
+      <c r="K44" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L44" t="n">
+        <v>288</v>
+      </c>
+      <c r="M44" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N44" t="n">
+        <v>1</v>
+      </c>
+      <c r="O44" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P44" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>15892</v>
+      </c>
+      <c r="R44" t="n">
+        <v>1</v>
+      </c>
+      <c r="S44" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -1618,6 +3092,39 @@
       <c r="H45" t="n">
         <v>50</v>
       </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" t="n">
+        <v>3</v>
+      </c>
+      <c r="K45" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L45" t="n">
+        <v>288</v>
+      </c>
+      <c r="M45" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N45" t="n">
+        <v>1</v>
+      </c>
+      <c r="O45" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P45" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>15892</v>
+      </c>
+      <c r="R45" t="n">
+        <v>1</v>
+      </c>
+      <c r="S45" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -1644,6 +3151,39 @@
       <c r="H46" t="n">
         <v>100</v>
       </c>
+      <c r="I46" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" t="n">
+        <v>3</v>
+      </c>
+      <c r="K46" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L46" t="n">
+        <v>288</v>
+      </c>
+      <c r="M46" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N46" t="n">
+        <v>1</v>
+      </c>
+      <c r="O46" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P46" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>15892</v>
+      </c>
+      <c r="R46" t="n">
+        <v>1</v>
+      </c>
+      <c r="S46" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -1670,6 +3210,39 @@
       <c r="H47" t="n">
         <v>200</v>
       </c>
+      <c r="I47" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" t="n">
+        <v>3</v>
+      </c>
+      <c r="K47" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L47" t="n">
+        <v>288</v>
+      </c>
+      <c r="M47" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N47" t="n">
+        <v>1</v>
+      </c>
+      <c r="O47" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P47" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>15892</v>
+      </c>
+      <c r="R47" t="n">
+        <v>1</v>
+      </c>
+      <c r="S47" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -1696,6 +3269,39 @@
       <c r="H48" t="n">
         <v>300</v>
       </c>
+      <c r="I48" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" t="n">
+        <v>3</v>
+      </c>
+      <c r="K48" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L48" t="n">
+        <v>288</v>
+      </c>
+      <c r="M48" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N48" t="n">
+        <v>1</v>
+      </c>
+      <c r="O48" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P48" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q48" t="n">
+        <v>15892</v>
+      </c>
+      <c r="R48" t="n">
+        <v>1</v>
+      </c>
+      <c r="S48" t="n">
+        <v>300</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -1722,6 +3328,39 @@
       <c r="H49" t="n">
         <v>500</v>
       </c>
+      <c r="I49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" t="n">
+        <v>3</v>
+      </c>
+      <c r="K49" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L49" t="n">
+        <v>288</v>
+      </c>
+      <c r="M49" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N49" t="n">
+        <v>1</v>
+      </c>
+      <c r="O49" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P49" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>15892</v>
+      </c>
+      <c r="R49" t="n">
+        <v>1</v>
+      </c>
+      <c r="S49" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -1748,6 +3387,39 @@
       <c r="H50" t="n">
         <v>1000</v>
       </c>
+      <c r="I50" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" t="n">
+        <v>3</v>
+      </c>
+      <c r="K50" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L50" t="n">
+        <v>288</v>
+      </c>
+      <c r="M50" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N50" t="n">
+        <v>1</v>
+      </c>
+      <c r="O50" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P50" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q50" t="n">
+        <v>15892</v>
+      </c>
+      <c r="R50" t="n">
+        <v>1</v>
+      </c>
+      <c r="S50" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -1774,6 +3446,39 @@
       <c r="H51" t="n">
         <v>1</v>
       </c>
+      <c r="I51" t="n">
+        <v>12101</v>
+      </c>
+      <c r="J51" t="n">
+        <v>3</v>
+      </c>
+      <c r="K51" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L51" t="n">
+        <v>288</v>
+      </c>
+      <c r="M51" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N51" t="n">
+        <v>1</v>
+      </c>
+      <c r="O51" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P51" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q51" t="n">
+        <v>15892</v>
+      </c>
+      <c r="R51" t="n">
+        <v>2</v>
+      </c>
+      <c r="S51" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -1800,6 +3505,39 @@
       <c r="H52" t="n">
         <v>50</v>
       </c>
+      <c r="I52" t="n">
+        <v>514400</v>
+      </c>
+      <c r="J52" t="n">
+        <v>3</v>
+      </c>
+      <c r="K52" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L52" t="n">
+        <v>288</v>
+      </c>
+      <c r="M52" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N52" t="n">
+        <v>1</v>
+      </c>
+      <c r="O52" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P52" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q52" t="n">
+        <v>15892</v>
+      </c>
+      <c r="R52" t="n">
+        <v>2</v>
+      </c>
+      <c r="S52" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -1826,6 +3564,39 @@
       <c r="H53" t="n">
         <v>100</v>
       </c>
+      <c r="I53" t="n">
+        <v>963200</v>
+      </c>
+      <c r="J53" t="n">
+        <v>3</v>
+      </c>
+      <c r="K53" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L53" t="n">
+        <v>288</v>
+      </c>
+      <c r="M53" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N53" t="n">
+        <v>1</v>
+      </c>
+      <c r="O53" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P53" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q53" t="n">
+        <v>15892</v>
+      </c>
+      <c r="R53" t="n">
+        <v>2</v>
+      </c>
+      <c r="S53" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -1852,6 +3623,39 @@
       <c r="H54" t="n">
         <v>200</v>
       </c>
+      <c r="I54" t="n">
+        <v>1904800</v>
+      </c>
+      <c r="J54" t="n">
+        <v>3</v>
+      </c>
+      <c r="K54" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L54" t="n">
+        <v>288</v>
+      </c>
+      <c r="M54" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N54" t="n">
+        <v>1</v>
+      </c>
+      <c r="O54" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P54" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q54" t="n">
+        <v>15892</v>
+      </c>
+      <c r="R54" t="n">
+        <v>2</v>
+      </c>
+      <c r="S54" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -1878,6 +3682,39 @@
       <c r="H55" t="n">
         <v>300</v>
       </c>
+      <c r="I55" t="n">
+        <v>2802000</v>
+      </c>
+      <c r="J55" t="n">
+        <v>3</v>
+      </c>
+      <c r="K55" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L55" t="n">
+        <v>288</v>
+      </c>
+      <c r="M55" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N55" t="n">
+        <v>1</v>
+      </c>
+      <c r="O55" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P55" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q55" t="n">
+        <v>15892</v>
+      </c>
+      <c r="R55" t="n">
+        <v>2</v>
+      </c>
+      <c r="S55" t="n">
+        <v>300</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -1904,6 +3741,39 @@
       <c r="H56" t="n">
         <v>500</v>
       </c>
+      <c r="I56" t="n">
+        <v>4532500</v>
+      </c>
+      <c r="J56" t="n">
+        <v>3</v>
+      </c>
+      <c r="K56" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L56" t="n">
+        <v>288</v>
+      </c>
+      <c r="M56" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N56" t="n">
+        <v>1</v>
+      </c>
+      <c r="O56" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P56" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q56" t="n">
+        <v>15892</v>
+      </c>
+      <c r="R56" t="n">
+        <v>2</v>
+      </c>
+      <c r="S56" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -1928,6 +3798,641 @@
         <v>2</v>
       </c>
       <c r="H57" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I57" t="n">
+        <v>8877000</v>
+      </c>
+      <c r="J57" t="n">
+        <v>3</v>
+      </c>
+      <c r="K57" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L57" t="n">
+        <v>288</v>
+      </c>
+      <c r="M57" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N57" t="n">
+        <v>1</v>
+      </c>
+      <c r="O57" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P57" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q57" t="n">
+        <v>15892</v>
+      </c>
+      <c r="R57" t="n">
+        <v>2</v>
+      </c>
+      <c r="S57" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr"/>
+      <c r="B58" t="inlineStr"/>
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="inlineStr"/>
+      <c r="E58" t="inlineStr"/>
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" t="n">
+        <v>3</v>
+      </c>
+      <c r="K58" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L58" t="n">
+        <v>288</v>
+      </c>
+      <c r="M58" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N58" t="n">
+        <v>1</v>
+      </c>
+      <c r="O58" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P58" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q58" t="n">
+        <v>15893</v>
+      </c>
+      <c r="R58" t="n">
+        <v>1</v>
+      </c>
+      <c r="S58" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr"/>
+      <c r="B59" t="inlineStr"/>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr"/>
+      <c r="E59" t="inlineStr"/>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="inlineStr"/>
+      <c r="H59" t="inlineStr"/>
+      <c r="I59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J59" t="n">
+        <v>3</v>
+      </c>
+      <c r="K59" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L59" t="n">
+        <v>288</v>
+      </c>
+      <c r="M59" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N59" t="n">
+        <v>1</v>
+      </c>
+      <c r="O59" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P59" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q59" t="n">
+        <v>15893</v>
+      </c>
+      <c r="R59" t="n">
+        <v>1</v>
+      </c>
+      <c r="S59" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr"/>
+      <c r="B60" t="inlineStr"/>
+      <c r="C60" t="inlineStr"/>
+      <c r="D60" t="inlineStr"/>
+      <c r="E60" t="inlineStr"/>
+      <c r="F60" t="inlineStr"/>
+      <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J60" t="n">
+        <v>3</v>
+      </c>
+      <c r="K60" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L60" t="n">
+        <v>288</v>
+      </c>
+      <c r="M60" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N60" t="n">
+        <v>1</v>
+      </c>
+      <c r="O60" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P60" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q60" t="n">
+        <v>15893</v>
+      </c>
+      <c r="R60" t="n">
+        <v>1</v>
+      </c>
+      <c r="S60" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr"/>
+      <c r="B61" t="inlineStr"/>
+      <c r="C61" t="inlineStr"/>
+      <c r="D61" t="inlineStr"/>
+      <c r="E61" t="inlineStr"/>
+      <c r="F61" t="inlineStr"/>
+      <c r="G61" t="inlineStr"/>
+      <c r="H61" t="inlineStr"/>
+      <c r="I61" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" t="n">
+        <v>3</v>
+      </c>
+      <c r="K61" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L61" t="n">
+        <v>288</v>
+      </c>
+      <c r="M61" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N61" t="n">
+        <v>1</v>
+      </c>
+      <c r="O61" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P61" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q61" t="n">
+        <v>15893</v>
+      </c>
+      <c r="R61" t="n">
+        <v>1</v>
+      </c>
+      <c r="S61" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr"/>
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" t="inlineStr"/>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="inlineStr"/>
+      <c r="H62" t="inlineStr"/>
+      <c r="I62" t="n">
+        <v>0</v>
+      </c>
+      <c r="J62" t="n">
+        <v>3</v>
+      </c>
+      <c r="K62" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L62" t="n">
+        <v>288</v>
+      </c>
+      <c r="M62" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N62" t="n">
+        <v>1</v>
+      </c>
+      <c r="O62" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P62" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q62" t="n">
+        <v>15893</v>
+      </c>
+      <c r="R62" t="n">
+        <v>1</v>
+      </c>
+      <c r="S62" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr"/>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" t="inlineStr"/>
+      <c r="H63" t="inlineStr"/>
+      <c r="I63" t="n">
+        <v>0</v>
+      </c>
+      <c r="J63" t="n">
+        <v>3</v>
+      </c>
+      <c r="K63" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L63" t="n">
+        <v>288</v>
+      </c>
+      <c r="M63" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N63" t="n">
+        <v>1</v>
+      </c>
+      <c r="O63" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P63" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q63" t="n">
+        <v>15893</v>
+      </c>
+      <c r="R63" t="n">
+        <v>1</v>
+      </c>
+      <c r="S63" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr"/>
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr"/>
+      <c r="E64" t="inlineStr"/>
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="inlineStr"/>
+      <c r="H64" t="inlineStr"/>
+      <c r="I64" t="n">
+        <v>0</v>
+      </c>
+      <c r="J64" t="n">
+        <v>3</v>
+      </c>
+      <c r="K64" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L64" t="n">
+        <v>288</v>
+      </c>
+      <c r="M64" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N64" t="n">
+        <v>1</v>
+      </c>
+      <c r="O64" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P64" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q64" t="n">
+        <v>15893</v>
+      </c>
+      <c r="R64" t="n">
+        <v>1</v>
+      </c>
+      <c r="S64" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr"/>
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr"/>
+      <c r="E65" t="inlineStr"/>
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr"/>
+      <c r="H65" t="inlineStr"/>
+      <c r="I65" t="n">
+        <v>21288</v>
+      </c>
+      <c r="J65" t="n">
+        <v>3</v>
+      </c>
+      <c r="K65" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L65" t="n">
+        <v>288</v>
+      </c>
+      <c r="M65" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N65" t="n">
+        <v>1</v>
+      </c>
+      <c r="O65" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P65" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q65" t="n">
+        <v>15893</v>
+      </c>
+      <c r="R65" t="n">
+        <v>2</v>
+      </c>
+      <c r="S65" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr"/>
+      <c r="B66" t="inlineStr"/>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="inlineStr"/>
+      <c r="E66" t="inlineStr"/>
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="inlineStr"/>
+      <c r="H66" t="inlineStr"/>
+      <c r="I66" t="n">
+        <v>891750</v>
+      </c>
+      <c r="J66" t="n">
+        <v>3</v>
+      </c>
+      <c r="K66" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L66" t="n">
+        <v>288</v>
+      </c>
+      <c r="M66" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N66" t="n">
+        <v>1</v>
+      </c>
+      <c r="O66" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P66" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q66" t="n">
+        <v>15893</v>
+      </c>
+      <c r="R66" t="n">
+        <v>2</v>
+      </c>
+      <c r="S66" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr"/>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr"/>
+      <c r="E67" t="inlineStr"/>
+      <c r="F67" t="inlineStr"/>
+      <c r="G67" t="inlineStr"/>
+      <c r="H67" t="inlineStr"/>
+      <c r="I67" t="n">
+        <v>1697600</v>
+      </c>
+      <c r="J67" t="n">
+        <v>3</v>
+      </c>
+      <c r="K67" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L67" t="n">
+        <v>288</v>
+      </c>
+      <c r="M67" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N67" t="n">
+        <v>1</v>
+      </c>
+      <c r="O67" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P67" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q67" t="n">
+        <v>15893</v>
+      </c>
+      <c r="R67" t="n">
+        <v>2</v>
+      </c>
+      <c r="S67" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr"/>
+      <c r="B68" t="inlineStr"/>
+      <c r="C68" t="inlineStr"/>
+      <c r="D68" t="inlineStr"/>
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="inlineStr"/>
+      <c r="G68" t="inlineStr"/>
+      <c r="H68" t="inlineStr"/>
+      <c r="I68" t="n">
+        <v>3372200</v>
+      </c>
+      <c r="J68" t="n">
+        <v>3</v>
+      </c>
+      <c r="K68" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L68" t="n">
+        <v>288</v>
+      </c>
+      <c r="M68" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N68" t="n">
+        <v>1</v>
+      </c>
+      <c r="O68" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P68" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q68" t="n">
+        <v>15893</v>
+      </c>
+      <c r="R68" t="n">
+        <v>2</v>
+      </c>
+      <c r="S68" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr"/>
+      <c r="B69" t="inlineStr"/>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr"/>
+      <c r="E69" t="inlineStr"/>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="inlineStr"/>
+      <c r="H69" t="inlineStr"/>
+      <c r="I69" t="n">
+        <v>4981500</v>
+      </c>
+      <c r="J69" t="n">
+        <v>3</v>
+      </c>
+      <c r="K69" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L69" t="n">
+        <v>288</v>
+      </c>
+      <c r="M69" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N69" t="n">
+        <v>1</v>
+      </c>
+      <c r="O69" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P69" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q69" t="n">
+        <v>15893</v>
+      </c>
+      <c r="R69" t="n">
+        <v>2</v>
+      </c>
+      <c r="S69" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr"/>
+      <c r="B70" t="inlineStr"/>
+      <c r="C70" t="inlineStr"/>
+      <c r="D70" t="inlineStr"/>
+      <c r="E70" t="inlineStr"/>
+      <c r="F70" t="inlineStr"/>
+      <c r="G70" t="inlineStr"/>
+      <c r="H70" t="inlineStr"/>
+      <c r="I70" t="n">
+        <v>8221500</v>
+      </c>
+      <c r="J70" t="n">
+        <v>3</v>
+      </c>
+      <c r="K70" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L70" t="n">
+        <v>288</v>
+      </c>
+      <c r="M70" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N70" t="n">
+        <v>1</v>
+      </c>
+      <c r="O70" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P70" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q70" t="n">
+        <v>15893</v>
+      </c>
+      <c r="R70" t="n">
+        <v>2</v>
+      </c>
+      <c r="S70" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr"/>
+      <c r="B71" t="inlineStr"/>
+      <c r="C71" t="inlineStr"/>
+      <c r="D71" t="inlineStr"/>
+      <c r="E71" t="inlineStr"/>
+      <c r="F71" t="inlineStr"/>
+      <c r="G71" t="inlineStr"/>
+      <c r="H71" t="inlineStr"/>
+      <c r="I71" t="n">
+        <v>16336000</v>
+      </c>
+      <c r="J71" t="n">
+        <v>3</v>
+      </c>
+      <c r="K71" t="n">
+        <v>1518</v>
+      </c>
+      <c r="L71" t="n">
+        <v>288</v>
+      </c>
+      <c r="M71" t="n">
+        <v>2399</v>
+      </c>
+      <c r="N71" t="n">
+        <v>1</v>
+      </c>
+      <c r="O71" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P71" t="n">
+        <v>1122</v>
+      </c>
+      <c r="Q71" t="n">
+        <v>15893</v>
+      </c>
+      <c r="R71" t="n">
+        <v>2</v>
+      </c>
+      <c r="S71" t="n">
         <v>1000</v>
       </c>
     </row>

</xml_diff>